<commit_message>
Updated presentation, and updated cost/timeline/risk sheet
</commit_message>
<xml_diff>
--- a/Project Documents/rotary kiln control upgrade cost - phase 1.xlsx
+++ b/Project Documents/rotary kiln control upgrade cost - phase 1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="96" windowWidth="22020" windowHeight="10056"/>
+    <workbookView xWindow="96" yWindow="156" windowWidth="22020" windowHeight="9996"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>HC 900 controller</t>
   </si>
@@ -30,25 +30,91 @@
     <t>Wiring</t>
   </si>
   <si>
-    <t>Brass tubing - pressure sensors</t>
-  </si>
-  <si>
     <t>Pressure transducers</t>
   </si>
   <si>
     <t>Thermocouples</t>
   </si>
   <si>
-    <t>Control Station Box</t>
-  </si>
-  <si>
-    <t>What else?</t>
-  </si>
-  <si>
     <t>Conduit</t>
   </si>
   <si>
     <t>John Clause Labor</t>
+  </si>
+  <si>
+    <t>Temperature display</t>
+  </si>
+  <si>
+    <t>copper tubing - pressure sensors</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Part Lead Time</t>
+  </si>
+  <si>
+    <t>Project Submission/Approval</t>
+  </si>
+  <si>
+    <t>Installation</t>
+  </si>
+  <si>
+    <t>Rotary kiln pressure control testing</t>
+  </si>
+  <si>
+    <t>Dryer system control testing</t>
+  </si>
+  <si>
+    <t>Weeks</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>weeks</t>
+  </si>
+  <si>
+    <t>Ceramic tube insert</t>
+  </si>
+  <si>
+    <t>Replacement damper &amp; actuator</t>
+  </si>
+  <si>
+    <t>West &amp; North gate actuators</t>
+  </si>
+  <si>
+    <t>Inst</t>
+  </si>
+  <si>
+    <t>Project Risks</t>
+  </si>
+  <si>
+    <t>Controller Setup Improperly</t>
+  </si>
+  <si>
+    <t>Response</t>
+  </si>
+  <si>
+    <t>Work closely with John Clause to ensure proper implementation. Confer with Tim Hastings as back-up check.</t>
+  </si>
+  <si>
+    <t>Almost impossible, as we are manually managing process control now (poorly.) Worst case is controller failure after comissioning. In this worst case, we can always go back to manual control.</t>
+  </si>
+  <si>
+    <t>Negative Impact on Production</t>
+  </si>
+  <si>
+    <t>Delay of Project Implementation due to maintenance unavailability</t>
+  </si>
+  <si>
+    <t>Option to outsource electrical work. Will add cost to the project. Alternatively, accept delays</t>
+  </si>
+  <si>
+    <t>Delay of Project due to production not running</t>
+  </si>
+  <si>
+    <t>This is a reality we must accept. Will work with Chandra to give input on best times to run for project, but ultimately production comes first.</t>
   </si>
 </sst>
 </file>
@@ -83,7 +149,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -91,14 +157,261 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,97 +713,298 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B34" sqref="A30:G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B1" s="5">
         <f>10680-B2</f>
         <v>7175</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="7">
         <f>3127+378</f>
         <v>3505</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="7">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="7">
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="7">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="7">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="7">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="7">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1">
-        <f>10*150</f>
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B10" s="7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="7">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="9">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="11">
+        <f>SUM(B1:B13)</f>
+        <v>23605</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="3"/>
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B19" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21">
         <v>5</v>
       </c>
-      <c r="B4" s="1">
-        <f>11*275</f>
-        <v>3025</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23">
         <v>4</v>
       </c>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="B27" s="1">
+        <f>SUM(B20:B26)</f>
+        <v>21</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="14"/>
+    </row>
+    <row r="31" spans="1:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="17"/>
+    </row>
+    <row r="32" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="19"/>
+    </row>
+    <row r="33" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="19"/>
+    </row>
+    <row r="34" spans="1:7" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="23"/>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B30:G30"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>